<commit_message>
Refactoring with finalised IDs across all classified EVEs
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-side-data.xlsx
+++ b/tabular/eve/ehbv-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE98DDD6-3AB0-CE4D-9167-BAE3179CC6FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE89E696-55FD-F348-A0DD-61FE77693ADB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10312,8 +10312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF929"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AF811"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AH30" sqref="AH30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>